<commit_message>
contact point label added
</commit_message>
<xml_diff>
--- a/source/ControlledTerms.xlsx
+++ b/source/ControlledTerms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birk/Documents/Jobs/SAPA/Development/spa-vocabulary/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CE7923-5A15-4C45-A9F3-5E34FC165503}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9301AA-9DE1-B84B-9376-EAA51863A432}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5860" yWindow="2980" windowWidth="44300" windowHeight="26580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,7 +340,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="1235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="1237">
   <si>
     <t>identifier</t>
   </si>
@@ -4045,6 +4045,12 @@
   </si>
   <si>
     <t>e-mail</t>
+  </si>
+  <si>
+    <t>contact point</t>
+  </si>
+  <si>
+    <t>Kontakt</t>
   </si>
 </sst>
 </file>
@@ -4592,7 +4598,7 @@
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4931,10 +4937,14 @@
       <c r="D13" s="23" t="s">
         <v>1225</v>
       </c>
-      <c r="I13" s="10"/>
+      <c r="I13" s="10" t="s">
+        <v>1235</v>
+      </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="L13" s="10" t="s">
+        <v>1236</v>
+      </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>

</xml_diff>